<commit_message>
GHD Befragung data renamed
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_Cooling_PenetrationRate.xlsx
+++ b/projects/test_building/input/Scenario_Cooling_PenetrationRate.xlsx
@@ -211,7 +211,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -263,7 +263,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,8 +622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
2009 values are added to cooling and ventilation availability tables
</commit_message>
<xml_diff>
--- a/projects/test_building/input/Scenario_Cooling_PenetrationRate.xlsx
+++ b/projects/test_building/input/Scenario_Cooling_PenetrationRate.xlsx
@@ -1,43 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yus\Documents\code\3E\RenderNew\projects\test_building\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/songminyu/Documents/Code/3E/RenderNew/projects/test_building/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29B7E3F7-EEA1-CA42-A7AF-6A1EC428C76C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="765" windowWidth="30240" windowHeight="17355"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="4" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Yu, Songmin</author>
   </authors>
   <commentList>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -45,7 +33,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Yu, Songmin:</t>
         </r>
@@ -54,7 +42,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 Based on GHD-Befragung data, the penetration rate of tertiary sectors in 2019 was inserted. Then, the other years are calculated by using the same values, as a temperoral solution.</t>
@@ -66,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="47">
   <si>
     <t>id_region</t>
   </si>
@@ -204,12 +192,15 @@
   </si>
   <si>
     <t>2050</t>
+  </si>
+  <si>
+    <t>2009</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -231,14 +222,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -282,54 +273,55 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A1:AS18" totalsRowShown="0">
-  <autoFilter ref="A1:AS18"/>
-  <tableColumns count="45">
-    <tableColumn id="1" name="id_region"/>
-    <tableColumn id="3" name="id_sector"/>
-    <tableColumn id="4" name="id_subsector"/>
-    <tableColumn id="6" name="unit"/>
-    <tableColumn id="7" name="2010"/>
-    <tableColumn id="8" name="2011"/>
-    <tableColumn id="9" name="2012"/>
-    <tableColumn id="10" name="2013"/>
-    <tableColumn id="11" name="2014"/>
-    <tableColumn id="12" name="2015"/>
-    <tableColumn id="13" name="2016"/>
-    <tableColumn id="14" name="2017"/>
-    <tableColumn id="15" name="2018"/>
-    <tableColumn id="16" name="2019"/>
-    <tableColumn id="17" name="2020"/>
-    <tableColumn id="2" name="2021"/>
-    <tableColumn id="18" name="2022"/>
-    <tableColumn id="19" name="2023"/>
-    <tableColumn id="20" name="2024"/>
-    <tableColumn id="21" name="2025"/>
-    <tableColumn id="22" name="2026"/>
-    <tableColumn id="23" name="2027"/>
-    <tableColumn id="24" name="2028"/>
-    <tableColumn id="25" name="2029"/>
-    <tableColumn id="26" name="2030"/>
-    <tableColumn id="27" name="2031"/>
-    <tableColumn id="28" name="2032"/>
-    <tableColumn id="29" name="2033"/>
-    <tableColumn id="30" name="2034"/>
-    <tableColumn id="31" name="2035"/>
-    <tableColumn id="32" name="2036"/>
-    <tableColumn id="33" name="2037"/>
-    <tableColumn id="34" name="2038"/>
-    <tableColumn id="35" name="2039"/>
-    <tableColumn id="36" name="2040"/>
-    <tableColumn id="37" name="2041"/>
-    <tableColumn id="38" name="2042"/>
-    <tableColumn id="39" name="2043"/>
-    <tableColumn id="40" name="2044"/>
-    <tableColumn id="41" name="2045"/>
-    <tableColumn id="42" name="2046"/>
-    <tableColumn id="43" name="2047"/>
-    <tableColumn id="44" name="2048"/>
-    <tableColumn id="45" name="2049"/>
-    <tableColumn id="46" name="2050"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table3" displayName="Table3" ref="A1:AT18" totalsRowShown="0">
+  <autoFilter ref="A1:AT18" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <tableColumns count="46">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="id_region"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="id_sector"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="id_subsector"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="unit"/>
+    <tableColumn id="5" xr3:uid="{301F77C5-AC2E-0F4F-8DA5-18331E51F64A}" name="2009"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="2010"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="2011"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="2012"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="2013"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="2014"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="2015"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="2016"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="2017"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="2018"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="2019"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="2020"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="2021"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="2022"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="2023"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="2024"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="2025"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="2026"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="2027"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="2028"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="2029"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="2030"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="2031"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="2032"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="2033"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="2034"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="2035"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="2036"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="2037"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="2038"/>
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="2039"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="2040"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="2041"/>
+    <tableColumn id="38" xr3:uid="{00000000-0010-0000-0000-000026000000}" name="2042"/>
+    <tableColumn id="39" xr3:uid="{00000000-0010-0000-0000-000027000000}" name="2043"/>
+    <tableColumn id="40" xr3:uid="{00000000-0010-0000-0000-000028000000}" name="2044"/>
+    <tableColumn id="41" xr3:uid="{00000000-0010-0000-0000-000029000000}" name="2045"/>
+    <tableColumn id="42" xr3:uid="{00000000-0010-0000-0000-00002A000000}" name="2046"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="2047"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="2048"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="2049"/>
+    <tableColumn id="46" xr3:uid="{00000000-0010-0000-0000-00002E000000}" name="2050"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -619,20 +611,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AT18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -646,130 +638,133 @@
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>8</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>9</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>10</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>12</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>4</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>5</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>6</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" t="s">
+      <c r="AL1" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" t="s">
+      <c r="AM1" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" t="s">
+      <c r="AN1" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" t="s">
+      <c r="AO1" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" t="s">
+      <c r="AP1" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" t="s">
+      <c r="AQ1" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" t="s">
+      <c r="AR1" t="s">
         <v>43</v>
       </c>
-      <c r="AR1" t="s">
+      <c r="AS1" t="s">
         <v>44</v>
       </c>
-      <c r="AS1" t="s">
+      <c r="AT1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>9</v>
       </c>
@@ -905,8 +900,11 @@
       <c r="AS2">
         <v>0.13953488372093023</v>
       </c>
+      <c r="AT2">
+        <v>0.13953488372093023</v>
+      </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>9</v>
       </c>
@@ -1042,8 +1040,11 @@
       <c r="AS3">
         <v>0.23631840796019901</v>
       </c>
+      <c r="AT3">
+        <v>0.23631840796019901</v>
+      </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>9</v>
       </c>
@@ -1179,8 +1180,11 @@
       <c r="AS4">
         <v>0.10849056603773585</v>
       </c>
+      <c r="AT4">
+        <v>0.10849056603773585</v>
+      </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>9</v>
       </c>
@@ -1316,8 +1320,11 @@
       <c r="AS5">
         <v>0.18345323741007194</v>
       </c>
+      <c r="AT5">
+        <v>0.18345323741007194</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>9</v>
       </c>
@@ -1453,8 +1460,11 @@
       <c r="AS6">
         <v>9.5238095238095233E-2</v>
       </c>
+      <c r="AT6">
+        <v>9.5238095238095233E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>9</v>
       </c>
@@ -1590,8 +1600,11 @@
       <c r="AS7">
         <v>0.19444444444444445</v>
       </c>
+      <c r="AT7">
+        <v>0.19444444444444445</v>
+      </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>9</v>
       </c>
@@ -1727,8 +1740,11 @@
       <c r="AS8">
         <v>0.19047619047619047</v>
       </c>
+      <c r="AT8">
+        <v>0.19047619047619047</v>
+      </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1864,8 +1880,11 @@
       <c r="AS9">
         <v>0.26415094339622641</v>
       </c>
+      <c r="AT9">
+        <v>0.26415094339622641</v>
+      </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2001,8 +2020,11 @@
       <c r="AS10">
         <v>0.15384615384615385</v>
       </c>
+      <c r="AT10">
+        <v>0.15384615384615385</v>
+      </c>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -2138,8 +2160,11 @@
       <c r="AS11">
         <v>0.12</v>
       </c>
+      <c r="AT11">
+        <v>0.12</v>
+      </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>9</v>
       </c>
@@ -2275,8 +2300,11 @@
       <c r="AS12">
         <v>0.11627906976744186</v>
       </c>
+      <c r="AT12">
+        <v>0.11627906976744186</v>
+      </c>
     </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2412,8 +2440,11 @@
       <c r="AS13">
         <v>0.1111111111111111</v>
       </c>
+      <c r="AT13">
+        <v>0.1111111111111111</v>
+      </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>9</v>
       </c>
@@ -2549,8 +2580,11 @@
       <c r="AS14">
         <v>0.16091954022988506</v>
       </c>
+      <c r="AT14">
+        <v>0.16091954022988506</v>
+      </c>
     </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>9</v>
       </c>
@@ -2686,8 +2720,11 @@
       <c r="AS15">
         <v>0.75</v>
       </c>
+      <c r="AT15">
+        <v>0.75</v>
+      </c>
     </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>9</v>
       </c>
@@ -2823,8 +2860,11 @@
       <c r="AS16">
         <v>0.19178082191780821</v>
       </c>
+      <c r="AT16">
+        <v>0.19178082191780821</v>
+      </c>
     </row>
-    <row r="17" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>9</v>
       </c>
@@ -2960,8 +3000,11 @@
       <c r="AS17">
         <v>0.12777777777777777</v>
       </c>
+      <c r="AT17">
+        <v>0.12777777777777777</v>
+      </c>
     </row>
-    <row r="18" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:46" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>9</v>
       </c>
@@ -2990,111 +3033,114 @@
         <v>0</v>
       </c>
       <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
         <v>7.3322916666660187E-3</v>
       </c>
-      <c r="K18" s="1">
+      <c r="L18" s="1">
         <v>5.116614583333301E-2</v>
       </c>
-      <c r="L18" s="1">
+      <c r="M18" s="1">
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="M18" s="1">
+      <c r="N18" s="1">
         <v>0.13883385416666699</v>
       </c>
-      <c r="N18" s="1">
+      <c r="O18" s="1">
         <v>0.17985792451167901</v>
       </c>
-      <c r="O18" s="1">
+      <c r="P18" s="1">
         <v>0.21774464279575501</v>
       </c>
-      <c r="P18" s="1">
+      <c r="Q18" s="1">
         <v>0.25229794713138698</v>
       </c>
-      <c r="Q18" s="1">
+      <c r="R18" s="1">
         <v>0.28344609665729997</v>
       </c>
-      <c r="R18" s="1">
+      <c r="S18" s="1">
         <v>0.31122621734150202</v>
       </c>
-      <c r="S18" s="1">
+      <c r="T18" s="1">
         <v>0.33576375772698802</v>
       </c>
-      <c r="T18" s="1">
+      <c r="U18" s="1">
         <v>0.35724998859891499</v>
       </c>
-      <c r="U18" s="1">
+      <c r="V18" s="1">
         <v>0.37592013726433399</v>
       </c>
-      <c r="V18" s="1">
+      <c r="W18" s="1">
         <v>0.39203395716294898</v>
       </c>
-      <c r="W18" s="1">
+      <c r="X18" s="1">
         <v>0.40585972251093699</v>
       </c>
-      <c r="X18" s="1">
+      <c r="Y18" s="1">
         <v>0.417661955825264</v>
       </c>
-      <c r="Y18" s="1">
+      <c r="Z18" s="1">
         <v>0.42769271037120399</v>
       </c>
-      <c r="Z18" s="1">
+      <c r="AA18" s="1">
         <v>0.43618594194480398</v>
       </c>
-      <c r="AA18" s="1">
+      <c r="AB18" s="1">
         <v>0.443354379693711</v>
       </c>
-      <c r="AB18" s="1">
+      <c r="AC18" s="1">
         <v>0.44938829534550101</v>
       </c>
-      <c r="AC18" s="1">
+      <c r="AD18" s="1">
         <v>0.45445562815274498</v>
       </c>
-      <c r="AD18" s="1">
+      <c r="AE18" s="1">
         <v>0.45870301293903898</v>
       </c>
-      <c r="AE18" s="1">
+      <c r="AF18" s="1">
         <v>0.46225735633096199</v>
       </c>
-      <c r="AF18" s="1">
+      <c r="AG18" s="1">
         <v>0.46522769721656199</v>
       </c>
-      <c r="AG18" s="1">
+      <c r="AH18" s="1">
         <v>0.467707164804191</v>
       </c>
-      <c r="AH18" s="1">
+      <c r="AI18" s="1">
         <v>0.46977490935872701</v>
       </c>
-      <c r="AI18" s="1">
+      <c r="AJ18" s="1">
         <v>0.471497927531278</v>
       </c>
-      <c r="AJ18" s="1">
+      <c r="AK18" s="1">
         <v>0.472932738254005</v>
       </c>
-      <c r="AK18" s="1">
+      <c r="AL18" s="1">
         <v>0.474126888931656</v>
       </c>
-      <c r="AL18" s="1">
+      <c r="AM18" s="1">
         <v>0.47512028752087099</v>
       </c>
-      <c r="AM18" s="1">
+      <c r="AN18" s="1">
         <v>0.475946366118216</v>
       </c>
-      <c r="AN18" s="1">
+      <c r="AO18" s="1">
         <v>0.47663308755242001</v>
       </c>
-      <c r="AO18" s="1">
+      <c r="AP18" s="1">
         <v>0.47720380948734198</v>
       </c>
-      <c r="AP18" s="1">
+      <c r="AQ18" s="1">
         <v>0.47767802165012602</v>
       </c>
-      <c r="AQ18" s="1">
+      <c r="AR18" s="1">
         <v>0.47807197169701698</v>
       </c>
-      <c r="AR18" s="1">
+      <c r="AS18" s="1">
         <v>0.478399194403275</v>
       </c>
-      <c r="AS18" s="1">
+      <c r="AT18" s="1">
         <v>0.47867095764534501</v>
       </c>
     </row>

</xml_diff>